<commit_message>
attribute names, 8.1.3 contents, checklist
</commit_message>
<xml_diff>
--- a/report/AML Submission Check Lists.xlsx
+++ b/report/AML Submission Check Lists.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17100" tabRatio="500"/>
+    <workbookView xWindow="-33520" yWindow="-8600" windowWidth="25600" windowHeight="17100" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="AML Submission" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="55">
   <si>
     <t>Number formatting of chapters is repeated:</t>
   </si>
@@ -148,6 +148,52 @@
   </si>
   <si>
     <t>?</t>
+  </si>
+  <si>
+    <t>&lt;property&gt; ::= [&lt;visibility&gt;] [‘/’] &lt;name&gt; [‘:’ &lt;prop-type&gt;] [‘[‘ &lt;multiplicity-range&gt; ‘]’] [‘=’ &lt;default&gt;] [‘{‘ &lt;prop-modifier &gt; [‘,’ &lt;prop-modifier &gt;]* ’}’]</t>
+  </si>
+  <si>
+    <t>&lt;ownedComment xmi:type='uml:Comment' xmi:id='_18_0_2_9cd0221_1415387037068_441145_10971' body='&amp;lt;html&amp;gt;&amp;#10;  &amp;lt;head&amp;gt;&amp;#10;&amp;#9;&amp;#9;&amp;lt;style&amp;gt;&amp;#10;&amp;#9;&amp;#9;&amp;#9;p {padding:0px; margin:0px;}&amp;#10;&amp;#9;&amp;#9;&amp;lt;/style&amp;gt;&amp;#10;&amp;#9;&amp;lt;/head&amp;gt;&amp;#10;  &amp;lt;body&amp;gt;&amp;#10;    &amp;lt;p&amp;gt;&amp;#10;The code system or code system or code system version that contained a description of the terminology code at the point in time it was referenced.&amp;#10;&amp;#10;    &amp;lt;/p&amp;gt;&amp;#10;&amp;#10;&amp;lt;/body&amp;gt;&amp;#10;&amp;lt;/html&amp;gt;'&gt;</t>
+  </si>
+  <si>
+    <t>&lt;annotatedElement xmi:idref='_18_0_2_9cd0221_1415314303371_203085_10072'/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/ownedComment&gt;</t>
+  </si>
+  <si>
+    <t>&lt;lowerValue xmi:type='uml:LiteralInteger' xmi:id='_18_0_2_9cd0221_1415314345979_807009_10074'/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;xmi:Extension extender='MagicDraw UML 18.0'&gt;</t>
+  </si>
+  <si>
+    <t>&lt;modelExtension&gt;</t>
+  </si>
+  <si>
+    <t>&lt;upperValue xmi:type='uml:LiteralUnlimitedNatural' xmi:id='_18_0_2_9cd0221_1415314345979_723586_10075' value='1'/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/modelExtension&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/xmi:Extension&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/ownedAttribute&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ownedAttribute xmi:type='uml:Property' xmi:id='_18_0_2_9cd0221_1415314303371_203085_10072' name='terminologyVersion' visibility='public' type='_18_0_2_9cd0221_1414186321748_769176_17132'&gt;
+      &lt;ownedComment xmi:type='uml:Comment' xmi:id='_18_0_2_9cd0221_1415387037068_441145_10971' body='&amp;lt;html&amp;gt;&amp;#10;  &amp;lt;head&amp;gt;&amp;#10;&amp;#9;&amp;#9;&amp;lt;style&amp;gt;&amp;#10;&amp;#9;&amp;#9;&amp;#9;p {padding:0px; margin:0px;}&amp;#10;&amp;#9;&amp;#9;&amp;lt;/style&amp;gt;&amp;#10;&amp;#9;&amp;lt;/head&amp;gt;&amp;#10;  &amp;lt;body&amp;gt;&amp;#10;    &amp;lt;p&amp;gt;&amp;#10;The code system or code system or code system version that contained a description of the terminology code at the point in time it was referenced.&amp;#10;&amp;#10;    &amp;lt;/p&amp;gt;&amp;#10;&amp;#10;&amp;lt;/body&amp;gt;&amp;#10;&amp;lt;/html&amp;gt;'&gt;
+       &lt;annotatedElement xmi:idref='_18_0_2_9cd0221_1415314303371_203085_10072'/&gt;
+      &lt;/ownedComment&gt;
+      &lt;lowerValue xmi:type='uml:LiteralInteger' xmi:id='_18_0_2_9cd0221_1415314345979_807009_10074'/&gt;
+      &lt;xmi:Extension extender='MagicDraw UML 18.0'&gt;
+       &lt;modelExtension&gt;
+        &lt;upperValue xmi:type='uml:LiteralUnlimitedNatural' xmi:id='_18_0_2_9cd0221_1415314345979_723586_10075' value='1'/&gt;
+       &lt;/modelExtension&gt;
+      &lt;/xmi:Extension&gt;
+     &lt;/ownedAttribute&gt;</t>
   </si>
 </sst>
 </file>
@@ -203,10 +249,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -543,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:O37"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -554,7 +603,8 @@
     <col min="1" max="1" width="5.83203125" customWidth="1"/>
     <col min="2" max="2" width="94.5" customWidth="1"/>
     <col min="3" max="5" width="10.83203125" style="1"/>
-    <col min="6" max="6" width="70" customWidth="1"/>
+    <col min="6" max="6" width="122.1640625" customWidth="1"/>
+    <col min="7" max="7" width="72.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -703,85 +753,148 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:15" ht="121" customHeight="1">
       <c r="A17" t="s">
         <v>15</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" t="s">
+        <v>43</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
       <c r="A18" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="D18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
       <c r="B19" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="D19" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="N19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
       <c r="A20" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="D20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
       <c r="A21" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="D21" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
       <c r="B22" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="D22" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
       <c r="A23" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="N23" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
       <c r="B24" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="O24" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15">
       <c r="A25" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="N25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
       <c r="A26" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="27" spans="1:4">
+      <c r="M26" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15">
       <c r="A27" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="L27" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15">
       <c r="A28" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:15">
       <c r="A29" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:15">
       <c r="A30" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:15">
       <c r="A31" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:15">
       <c r="A32" t="s">
         <v>30</v>
       </c>

</xml_diff>